<commit_message>
alterações referente a caixa e financeiro
</commit_message>
<xml_diff>
--- a/docs/ARTEFATOS(15-23)/Controlar_Fluxo_De_Caixa/Analise_de_Eventos_CONTROLAR_FLUXO_DE_CAIXA.xlsx
+++ b/docs/ARTEFATOS(15-23)/Controlar_Fluxo_De_Caixa/Analise_de_Eventos_CONTROLAR_FLUXO_DE_CAIXA.xlsx
@@ -9,7 +9,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7miSzS9muB8gzYOQTfrCRzpLknvICQ=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mioEKkwtZIlS1AhglfFxmpyrOvBgA=="/>
     </ext>
   </extLst>
 </workbook>
@@ -78,7 +78,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
@@ -99,10 +99,6 @@
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11.0"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -253,7 +249,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="26">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -304,28 +300,19 @@
     </xf>
     <xf borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf borderId="7" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="7" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="7" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="7" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="7" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="12" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="7" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -624,16 +611,16 @@
     <row r="4">
       <c r="A4" s="18"/>
       <c r="B4" s="19"/>
-      <c r="C4" s="20">
+      <c r="C4" s="12">
         <v>2.0</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="22"/>
+      <c r="E4" s="21"/>
       <c r="F4" s="14"/>
       <c r="G4" s="16"/>
-      <c r="H4" s="23" t="s">
+      <c r="H4" s="22" t="s">
         <v>14</v>
       </c>
       <c r="I4" s="16"/>
@@ -642,28 +629,28 @@
     <row r="5">
       <c r="A5" s="18"/>
       <c r="B5" s="19"/>
-      <c r="C5" s="20">
+      <c r="C5" s="12">
         <v>3.0</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24" t="s">
+      <c r="E5" s="21"/>
+      <c r="F5" s="21" t="s">
         <v>14</v>
       </c>
       <c r="G5" s="16"/>
-      <c r="H5" s="25"/>
+      <c r="H5" s="22"/>
       <c r="I5" s="16"/>
       <c r="J5" s="17"/>
     </row>
     <row r="6">
-      <c r="A6" s="26"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="20">
+      <c r="A6" s="23"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="12">
         <v>4.0</v>
       </c>
-      <c r="D6" s="28" t="s">
+      <c r="D6" s="25" t="s">
         <v>17</v>
       </c>
       <c r="E6" s="14"/>

</xml_diff>